<commit_message>
CPP code now supports multiple devices. Power is down on all units by default, turned on only during reset, to prevent large power consumption
</commit_message>
<xml_diff>
--- a/examples/EMTF_MPCX_full/src/protocol_MPCX.xlsx
+++ b/examples/EMTF_MPCX_full/src/protocol_MPCX.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MPCX_mgt_atts_notxbuf" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4110" uniqueCount="934">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4112" uniqueCount="936">
   <si>
     <t xml:space="preserve">//----------------RX</t>
   </si>
@@ -2736,6 +2736,12 @@
   </si>
   <si>
     <t xml:space="preserve">should be 4’b1010 for 800 mV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RXPD, TXPD,QPLLPD,CPLLPD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set all of these to all 1, to have power down by default</t>
   </si>
   <si>
     <t xml:space="preserve">If RXSLIDE is used, set the following:</t>
@@ -2968,8 +2974,8 @@
   </sheetPr>
   <dimension ref="A1:D710"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A388" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B405" activeCellId="1" sqref="B363 B405"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6255,7 +6261,7 @@
         <v>481</v>
       </c>
       <c r="B403" s="0" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C403" s="1"/>
     </row>
@@ -6264,7 +6270,7 @@
         <v>482</v>
       </c>
       <c r="B404" s="0" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C404" s="1"/>
     </row>
@@ -9038,8 +9044,8 @@
   </sheetPr>
   <dimension ref="A1:E710"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A348" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B363" activeCellId="0" sqref="B363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14957,7 +14963,7 @@
         <v>419</v>
       </c>
       <c r="B363" s="0" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C363" s="1" t="s">
         <v>419</v>
@@ -14967,7 +14973,7 @@
       </c>
       <c r="E363" s="0" t="str">
         <f aca="false">IF(B363&lt;&gt;D363,"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15677,7 +15683,7 @@
         <v>481</v>
       </c>
       <c r="B403" s="0" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C403" s="1" t="s">
         <v>481</v>
@@ -15687,7 +15693,7 @@
       </c>
       <c r="E403" s="0" t="str">
         <f aca="false">IF(B403&lt;&gt;D403,"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15695,7 +15701,7 @@
         <v>482</v>
       </c>
       <c r="B404" s="0" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C404" s="1" t="s">
         <v>482</v>
@@ -15705,7 +15711,7 @@
       </c>
       <c r="E404" s="0" t="str">
         <f aca="false">IF(B404&lt;&gt;D404,"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21228,8 +21234,8 @@
   </sheetPr>
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B363 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21730,8 +21736,8 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B363 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21799,16 +21805,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="1" sqref="B363 C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
   </cols>
   <sheetData>
@@ -21937,21 +21943,21 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="5" t="s">
         <v>904</v>
       </c>
+      <c r="D21" s="0" t="s">
+        <v>905</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="5" t="s">
-        <v>577</v>
-      </c>
-      <c r="D22" s="0" t="n">
-        <v>0</v>
+      <c r="B22" s="5" t="s">
+        <v>906</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="5" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>0</v>
@@ -21959,109 +21965,109 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="5" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="5" t="s">
+        <v>575</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="7" t="n">
+      <c r="D26" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
-        <v>905</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="6" t="s">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="6" t="s">
         <v>865</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D29" s="0" t="s">
         <v>895</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="0" t="s">
-        <v>829</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>906</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0" t="s">
+        <v>829</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="0" t="s">
         <v>832</v>
       </c>
-      <c r="D30" s="6" t="s">
-        <v>907</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>908</v>
-      </c>
-    </row>
+      <c r="D31" s="6" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
-        <v>909</v>
+      <c r="A33" s="0" t="s">
+        <v>910</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="0" t="s">
-        <v>912</v>
+      <c r="B36" s="0" t="s">
+        <v>913</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
-        <v>913</v>
+      <c r="C37" s="0" t="s">
+        <v>914</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
         <v>915</v>
       </c>
     </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="s">
+        <v>916</v>
+      </c>
+    </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="s">
-        <v>916</v>
+      <c r="A41" s="0" t="s">
+        <v>917</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>917</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="1" t="s">
         <v>918</v>
       </c>
-      <c r="D43" s="0" t="s">
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0" t="s">
         <v>919</v>
       </c>
     </row>
@@ -22119,6 +22125,14 @@
       </c>
       <c r="D50" s="0" t="s">
         <v>933</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C51" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>935</v>
       </c>
     </row>
   </sheetData>

</xml_diff>